<commit_message>
update git ignore and schedule
</commit_message>
<xml_diff>
--- a/data/schedule.xlsx
+++ b/data/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshuarosenberg/s21-intro-to-data-sci-methods-in-ed/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D51294-D902-3B44-8A73-0BC239A903EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5147F913-6192-1D42-88EC-179CB4F307A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{3759121A-71D8-DD43-A2AE-D807B9ADF3B0}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23360" windowHeight="21900" xr2:uid="{3759121A-71D8-DD43-A2AE-D807B9ADF3B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
   <si>
     <t>Date</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Homework</t>
   </si>
   <si>
-    <t>Assignment Due</t>
-  </si>
-  <si>
     <t>Week 1   - Jan 21</t>
   </si>
   <si>
@@ -84,9 +81,6 @@
     <t>HW3</t>
   </si>
   <si>
-    <t>Exam 1</t>
-  </si>
-  <si>
     <t>Week 4   - Feb 11</t>
   </si>
   <si>
@@ -96,9 +90,6 @@
     <t>HW4</t>
   </si>
   <si>
-    <t>Privacy Statement (Initial)</t>
-  </si>
-  <si>
     <t>Week 5   - Feb 18</t>
   </si>
   <si>
@@ -120,48 +111,27 @@
     <t>Week 7   - Mar 4</t>
   </si>
   <si>
-    <t>3: Ethics</t>
-  </si>
-  <si>
-    <t>Surveillance and privacy</t>
-  </si>
-  <si>
     <t>HW8</t>
   </si>
   <si>
-    <t>Exam 2</t>
-  </si>
-  <si>
     <t>Week 8   - Mar 11</t>
   </si>
   <si>
-    <t>Strategic (and not strategic) uses of data</t>
-  </si>
-  <si>
     <t>HW9</t>
   </si>
   <si>
     <t>Week 9   - Mar 18</t>
   </si>
   <si>
-    <t>Protecting anonymous data</t>
-  </si>
-  <si>
     <t>HW10</t>
   </si>
   <si>
     <t>Week 10 - Mar 25</t>
   </si>
   <si>
-    <t>4: Making conclusions</t>
-  </si>
-  <si>
     <t>Estimating parameters</t>
   </si>
   <si>
-    <t>Exam 3</t>
-  </si>
-  <si>
     <t>Week 11 - Apr 1</t>
   </si>
   <si>
@@ -204,7 +174,31 @@
     <t>HW14</t>
   </si>
   <si>
-    <t>Feedback on final presentations; Exam 4 </t>
+    <t>3: Drawing conclusions</t>
+  </si>
+  <si>
+    <t>Assignment</t>
+  </si>
+  <si>
+    <t>Exam</t>
+  </si>
+  <si>
+    <t>Color, stacking and dodging bars, and faceting</t>
+  </si>
+  <si>
+    <t>Summarizing data in tables</t>
+  </si>
+  <si>
+    <t>More on tables and a gentle introduction to modeling</t>
+  </si>
+  <si>
+    <t>Data ethics statement feedback</t>
+  </si>
+  <si>
+    <t>Data ethics statement (draft)</t>
+  </si>
+  <si>
+    <t>Revised data ethics statement; Feedback on final presentations</t>
   </si>
 </sst>
 </file>
@@ -246,8 +240,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -565,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2623079-2E11-B44C-BF66-2AA9439365FA}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -579,7 +575,7 @@
     <col min="4" max="4" width="45.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -593,205 +589,210 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="1" t="s">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="D7" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="D8" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="E9" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="C10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="E10" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E11" s="2"/>
+      <c r="F11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="B12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="D12" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="F15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>